<commit_message>
done some changes to the code and added functions to calculate memory usage. Updated data file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="74">
   <si>
     <t xml:space="preserve">Ubuntu </t>
   </si>
@@ -49,45 +49,48 @@
     <t xml:space="preserve">Time to calculate x</t>
   </si>
   <si>
+    <t xml:space="preserve">Memory before loading matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1641 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1729 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1731 MB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1733 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory after loading matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1644 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1729 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1731 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max memory usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++ EIGEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shallow_water1 [2.3 MB]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Memory before load matrix</t>
   </si>
   <si>
-    <t xml:space="preserve">1641 MB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1729 MB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1731 MB </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1733 MB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memory after loading matrix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1644 MB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1729 MB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1731 MB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max memory usage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relative error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C++ EIGEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shallow_water1 [2.3 MB]</t>
-  </si>
-  <si>
     <t xml:space="preserve">1770 MB</t>
   </si>
   <si>
@@ -233,6 +236,12 @@
   </si>
   <si>
     <t xml:space="preserve">AFTER 10H IT DIDN’T FINISHED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rivedere memoria usata da matlab in windows</t>
   </si>
 </sst>
 </file>
@@ -243,7 +252,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -274,6 +283,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -282,7 +297,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,7 +319,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFF200"/>
       </patternFill>
     </fill>
     <fill>
@@ -335,6 +350,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF59C5C7"/>
         <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -372,7 +393,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -417,6 +438,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -437,7 +462,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -451,6 +476,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -490,7 +519,7 @@
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -532,15 +561,15 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="16.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="1" width="16.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="0" width="16.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.55"/>
@@ -634,11 +663,11 @@
         <v>0.01580862115</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -667,7 +696,7 @@
       <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -686,36 +715,36 @@
       <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="12" t="n">
+      <c r="B8" s="13" t="n">
         <v>6.65034213505581E-007</v>
       </c>
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="13" t="n">
         <v>6.65034213505581E-007</v>
       </c>
-      <c r="D8" s="12" t="n">
+      <c r="D8" s="13" t="n">
         <v>6.65034213505581E-007</v>
       </c>
-      <c r="E8" s="12" t="n">
+      <c r="E8" s="13" t="n">
         <v>6.65034213505581E-007</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="13" t="n">
+      <c r="G8" s="14" t="n">
         <v>6.80303721118679E-007</v>
       </c>
-      <c r="H8" s="14" t="n">
+      <c r="H8" s="15" t="n">
         <v>6.80303721118679E-007</v>
       </c>
-      <c r="I8" s="13" t="n">
+      <c r="I8" s="14" t="n">
         <v>6.80303721118679E-007</v>
       </c>
-      <c r="J8" s="14" t="n">
+      <c r="J8" s="15" t="n">
         <v>6.80303721118679E-007</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -730,7 +759,7 @@
       <c r="E9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -751,26 +780,38 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.010731</v>
+        <v>0.251748</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0.010605</v>
+        <v>0.253653</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.010897</v>
+        <v>0.252379</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>0.010697</v>
+        <v>0.25219</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="B11" s="0" t="n">
+        <v>1980</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1996</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1996</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -778,15 +819,39 @@
       <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
+      <c r="B12" s="0" t="n">
+        <v>4824</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>4816</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4852</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>4828</v>
+      </c>
       <c r="F12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="11"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="B13" s="0" t="n">
+        <v>7628</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>7676</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>7656</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>7632</v>
+      </c>
       <c r="F13" s="10" t="s">
         <v>18</v>
       </c>
@@ -795,25 +860,25 @@
       <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="12" t="n">
+      <c r="B14" s="13" t="n">
         <v>8.84991E-007</v>
       </c>
-      <c r="C14" s="12" t="n">
+      <c r="C14" s="13" t="n">
         <v>8.84991E-007</v>
       </c>
-      <c r="D14" s="12" t="n">
+      <c r="D14" s="13" t="n">
         <v>8.84991E-007</v>
       </c>
-      <c r="E14" s="12" t="n">
+      <c r="E14" s="13" t="n">
         <v>8.84991E-007</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
@@ -889,22 +954,22 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>9</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,17 +979,17 @@
       <c r="F19" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="11" t="s">
+      <c r="G19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="I19" s="12" t="s">
         <v>28</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,36 +1004,36 @@
       <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="n">
+      <c r="B21" s="13" t="n">
         <v>2.37690352199598E-016</v>
       </c>
-      <c r="C21" s="12" t="n">
+      <c r="C21" s="13" t="n">
         <v>2.37690352199598E-016</v>
       </c>
-      <c r="D21" s="12" t="n">
+      <c r="D21" s="13" t="n">
         <v>2.37690352199598E-016</v>
       </c>
-      <c r="E21" s="12" t="n">
+      <c r="E21" s="13" t="n">
         <v>2.37690352199598E-016</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="12" t="n">
+      <c r="G21" s="13" t="n">
         <v>2.37690352199597E-016</v>
       </c>
-      <c r="H21" s="13" t="n">
+      <c r="H21" s="14" t="n">
         <v>2.37690352199597E-016</v>
       </c>
-      <c r="I21" s="13" t="n">
+      <c r="I21" s="14" t="n">
         <v>2.37690352199597E-016</v>
       </c>
-      <c r="J21" s="13" t="n">
+      <c r="J21" s="14" t="n">
         <v>2.37690352199597E-016</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -983,7 +1048,7 @@
       <c r="E22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G22" s="9" t="s">
@@ -1004,27 +1069,39 @@
         <v>8</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.1174</v>
+        <v>5.168093</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0.125128</v>
+        <v>5.264911</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0.117291</v>
+        <v>5.334158</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>0.116939</v>
+        <v>5.159856</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K23" s="16"/>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="B24" s="0" t="n">
+        <v>1908</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1820</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1908</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>1828</v>
+      </c>
+      <c r="F24" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1032,18 +1109,42 @@
       <c r="A25" s="10" t="s">
         <v>14</v>
       </c>
+      <c r="B25" s="0" t="n">
+        <v>9296</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>9264</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>9288</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>9116</v>
+      </c>
       <c r="F25" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="B26" s="0" t="n">
+        <v>39988</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>39892</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>39980</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>39872</v>
+      </c>
       <c r="F26" s="10" t="s">
         <v>18</v>
       </c>
@@ -1052,32 +1153,32 @@
       <c r="A27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="12" t="n">
+      <c r="B27" s="13" t="n">
         <v>2.77912E-016</v>
       </c>
-      <c r="C27" s="12" t="n">
+      <c r="C27" s="13" t="n">
         <v>2.77912E-016</v>
       </c>
-      <c r="D27" s="12" t="n">
+      <c r="D27" s="13" t="n">
         <v>2.77912E-016</v>
       </c>
-      <c r="E27" s="12" t="n">
+      <c r="E27" s="13" t="n">
         <v>2.77912E-016</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,23 +1246,23 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,17 +1272,17 @@
       <c r="F32" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="11" t="s">
-        <v>34</v>
+      <c r="G32" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,36 +1297,36 @@
       <c r="A34" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="12" t="n">
+      <c r="B34" s="13" t="n">
         <v>4.3712464003367E-011</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="13" t="n">
         <v>4.3712464003367E-011</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="13" t="n">
         <v>4.3712464003367E-011</v>
       </c>
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="13" t="n">
         <v>4.3712464003367E-011</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="12" t="n">
+      <c r="G34" s="13" t="n">
         <v>4.37410917936885E-011</v>
       </c>
-      <c r="H34" s="13" t="n">
+      <c r="H34" s="14" t="n">
         <v>4.37410917936885E-011</v>
       </c>
-      <c r="I34" s="13" t="n">
+      <c r="I34" s="14" t="n">
         <v>4.37410917936885E-011</v>
       </c>
-      <c r="J34" s="13" t="n">
+      <c r="J34" s="14" t="n">
         <v>4.37410917936885E-011</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -1240,7 +1341,7 @@
       <c r="E35" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G35" s="9" t="s">
@@ -1261,17 +1362,20 @@
         <v>8</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>6.312409</v>
+        <v>2387.52898</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="B37" s="0" t="n">
+        <v>1872</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1279,18 +1383,24 @@
       <c r="A38" s="10" t="s">
         <v>14</v>
       </c>
+      <c r="B38" s="0" t="n">
+        <v>55100</v>
+      </c>
       <c r="F38" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="B39" s="0" t="n">
+        <v>2716200</v>
+      </c>
       <c r="F39" s="10" t="s">
         <v>18</v>
       </c>
@@ -1299,26 +1409,26 @@
       <c r="A40" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="12" t="n">
+      <c r="B40" s="13" t="n">
         <v>7.65522E-011</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
       <c r="F40" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1360,7 +1470,7 @@
       <c r="B43" s="0" t="n">
         <v>1.6961926775</v>
       </c>
-      <c r="C43" s="12" t="n">
+      <c r="C43" s="13" t="n">
         <v>1.6782621775</v>
       </c>
       <c r="D43" s="0" t="n">
@@ -1375,7 +1485,7 @@
       <c r="G43" s="1" t="n">
         <v>1.7010531644</v>
       </c>
-      <c r="H43" s="13" t="n">
+      <c r="H43" s="14" t="n">
         <v>1.6956039644</v>
       </c>
       <c r="I43" s="1" t="n">
@@ -1386,23 +1496,23 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,16 +1523,16 @@
         <v>14</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,40 +1547,40 @@
       <c r="A47" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="12" t="n">
+      <c r="B47" s="13" t="n">
         <v>1.09185181855155E-012</v>
       </c>
-      <c r="C47" s="12" t="n">
+      <c r="C47" s="13" t="n">
         <v>1.09185181855155E-012</v>
       </c>
-      <c r="D47" s="12" t="n">
+      <c r="D47" s="13" t="n">
         <v>1.09185181855155E-012</v>
       </c>
-      <c r="E47" s="12" t="n">
+      <c r="E47" s="13" t="n">
         <v>1.09185181855155E-012</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G47" s="12" t="n">
+      <c r="G47" s="13" t="n">
         <v>1.08593319293648E-012</v>
       </c>
-      <c r="H47" s="13" t="n">
+      <c r="H47" s="14" t="n">
         <v>1.08593319293648E-012</v>
       </c>
-      <c r="I47" s="13" t="n">
+      <c r="I47" s="14" t="n">
         <v>1.08593319293648E-012</v>
       </c>
-      <c r="J47" s="13" t="n">
+      <c r="J47" s="14" t="n">
         <v>1.08593319293648E-012</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1512,13 +1622,13 @@
       <c r="B50" s="0" t="n">
         <v>8.3968946775</v>
       </c>
-      <c r="C50" s="12" t="n">
+      <c r="C50" s="13" t="n">
         <v>8.4139606775</v>
       </c>
-      <c r="D50" s="12" t="n">
+      <c r="D50" s="13" t="n">
         <v>8.4458086775</v>
       </c>
-      <c r="E50" s="12" t="n">
+      <c r="E50" s="13" t="n">
         <v>8.5108536775</v>
       </c>
       <c r="F50" s="10" t="s">
@@ -1527,34 +1637,34 @@
       <c r="G50" s="1" t="n">
         <v>9.6780539644</v>
       </c>
-      <c r="H50" s="13" t="n">
+      <c r="H50" s="14" t="n">
         <v>15.6523706644</v>
       </c>
-      <c r="I50" s="13" t="n">
+      <c r="I50" s="14" t="n">
         <v>10.3934736644</v>
       </c>
-      <c r="J50" s="13" t="n">
+      <c r="J50" s="14" t="n">
         <v>10.3519378644</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,16 +1675,16 @@
         <v>14</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1589,40 +1699,40 @@
       <c r="A54" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="12" t="n">
+      <c r="B54" s="13" t="n">
         <v>3.52055117278781E-012</v>
       </c>
-      <c r="C54" s="12" t="n">
+      <c r="C54" s="13" t="n">
         <v>3.52055117278781E-012</v>
       </c>
-      <c r="D54" s="12" t="n">
+      <c r="D54" s="13" t="n">
         <v>3.52055117278781E-012</v>
       </c>
-      <c r="E54" s="12" t="n">
+      <c r="E54" s="13" t="n">
         <v>3.52055117278781E-012</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G54" s="12" t="n">
+      <c r="G54" s="13" t="n">
         <v>3.52312377029344E-012</v>
       </c>
-      <c r="H54" s="13" t="n">
+      <c r="H54" s="14" t="n">
         <v>3.52312377029344E-012</v>
       </c>
-      <c r="I54" s="13" t="n">
+      <c r="I54" s="14" t="n">
         <v>3.52312377029344E-012</v>
       </c>
-      <c r="J54" s="13" t="n">
+      <c r="J54" s="14" t="n">
         <v>3.52312377029344E-012</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,13 +1774,13 @@
       <c r="B57" s="0" t="n">
         <v>0.9488136775</v>
       </c>
-      <c r="C57" s="12" t="n">
+      <c r="C57" s="13" t="n">
         <v>1.0271606775</v>
       </c>
-      <c r="D57" s="12" t="n">
+      <c r="D57" s="13" t="n">
         <v>0.9529426775</v>
       </c>
-      <c r="E57" s="12" t="n">
+      <c r="E57" s="13" t="n">
         <v>0.9631676775</v>
       </c>
       <c r="F57" s="10" t="s">
@@ -1679,34 +1789,34 @@
       <c r="G57" s="1" t="n">
         <v>1.1807083644</v>
       </c>
-      <c r="H57" s="13" t="n">
+      <c r="H57" s="14" t="n">
         <v>1.2784996644</v>
       </c>
-      <c r="I57" s="13" t="n">
+      <c r="I57" s="14" t="n">
         <v>1.1672463644</v>
       </c>
-      <c r="J57" s="13" t="n">
+      <c r="J57" s="14" t="n">
         <v>1.1704009644</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="F58" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,16 +1827,16 @@
         <v>14</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1741,40 +1851,40 @@
       <c r="A61" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="12" t="n">
+      <c r="B61" s="13" t="n">
         <v>1.24774344421239E-013</v>
       </c>
-      <c r="C61" s="12" t="n">
+      <c r="C61" s="13" t="n">
         <v>1.24774344421239E-013</v>
       </c>
-      <c r="D61" s="12" t="n">
+      <c r="D61" s="13" t="n">
         <v>1.24774344421239E-013</v>
       </c>
-      <c r="E61" s="12" t="n">
+      <c r="E61" s="13" t="n">
         <v>1.24774344421239E-013</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G61" s="12" t="n">
+      <c r="G61" s="13" t="n">
         <v>9.4510413200822E-014</v>
       </c>
-      <c r="H61" s="13" t="n">
+      <c r="H61" s="14" t="n">
         <v>9.4510413200822E-014</v>
       </c>
-      <c r="I61" s="13" t="n">
+      <c r="I61" s="14" t="n">
         <v>9.4510413200822E-014</v>
       </c>
-      <c r="J61" s="13" t="n">
+      <c r="J61" s="14" t="n">
         <v>9.4510413200822E-014</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,13 +1926,13 @@
       <c r="B64" s="0" t="n">
         <v>2.1868166775</v>
       </c>
-      <c r="C64" s="12" t="n">
+      <c r="C64" s="13" t="n">
         <v>2.1862206775</v>
       </c>
-      <c r="D64" s="12" t="n">
+      <c r="D64" s="13" t="n">
         <v>2.2231206775</v>
       </c>
-      <c r="E64" s="12" t="n">
+      <c r="E64" s="13" t="n">
         <v>2.1912646775</v>
       </c>
       <c r="F64" s="10" t="s">
@@ -1831,34 +1941,34 @@
       <c r="G64" s="1" t="n">
         <v>2.89429934875</v>
       </c>
-      <c r="H64" s="13" t="n">
+      <c r="H64" s="14" t="n">
         <v>2.99541039875</v>
       </c>
-      <c r="I64" s="13" t="n">
+      <c r="I64" s="14" t="n">
         <v>2.90823719875</v>
       </c>
-      <c r="J64" s="13" t="n">
+      <c r="J64" s="14" t="n">
         <v>2.95560069875</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,16 +1979,16 @@
         <v>14</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,47 +2003,47 @@
       <c r="A68" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B68" s="12" t="n">
+      <c r="B68" s="13" t="n">
         <v>3.92666580709667E-013</v>
       </c>
-      <c r="C68" s="12" t="n">
+      <c r="C68" s="13" t="n">
         <v>3.92666580709667E-013</v>
       </c>
-      <c r="D68" s="12" t="n">
+      <c r="D68" s="13" t="n">
         <v>3.92666580709667E-013</v>
       </c>
-      <c r="E68" s="12" t="n">
+      <c r="E68" s="13" t="n">
         <v>3.92666580709667E-013</v>
       </c>
       <c r="F68" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G68" s="12" t="n">
+      <c r="G68" s="13" t="n">
         <v>4.12976783068911E-013</v>
       </c>
-      <c r="H68" s="13" t="n">
+      <c r="H68" s="14" t="n">
         <v>4.12976783068911E-013</v>
       </c>
-      <c r="I68" s="13" t="n">
+      <c r="I68" s="14" t="n">
         <v>4.12976783068911E-013</v>
       </c>
-      <c r="J68" s="13" t="n">
+      <c r="J68" s="14" t="n">
         <v>4.12976783068911E-013</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B69" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="17"/>
+      <c r="B69" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="18"/>
       <c r="F69" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G69" s="17"/>
-      <c r="H69" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="G69" s="18"/>
+      <c r="H69" s="19"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7" t="s">
@@ -1971,21 +2081,21 @@
       <c r="A71" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
       <c r="F71" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F72" s="10" t="s">
+      <c r="F72" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2009,31 +2119,31 @@
       <c r="A75" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
       <c r="F75" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G75" s="12"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B76" s="17" t="s">
+      <c r="A76" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C76" s="17"/>
-      <c r="F76" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G76" s="17"/>
-      <c r="H76" s="18"/>
+      <c r="B76" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C76" s="18"/>
+      <c r="F76" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G76" s="18"/>
+      <c r="H76" s="19"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
@@ -2077,11 +2187,11 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B79" s="1"/>
-      <c r="F79" s="10" t="s">
+      <c r="F79" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2107,15 +2217,47 @@
       <c r="A82" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B82" s="12"/>
+      <c r="B82" s="13"/>
       <c r="F82" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G82" s="12"/>
+      <c r="G82" s="13"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B87" s="21"/>
+    </row>
+    <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B88" s="21"/>
+    </row>
+    <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="21"/>
+      <c r="B89" s="21"/>
+    </row>
+    <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+    </row>
+    <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="21"/>
+      <c r="B91" s="21"/>
+    </row>
+    <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+    </row>
+    <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="21"/>
+      <c r="B93" s="21"/>
+    </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added physical memory plots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,18 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carloradice\Documents\MCSLinearSystemSolver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918D0CA3-B6E1-4FDF-9074-AA82966EB748}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFE1029-288A-4610-8E49-894662F679B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">(Foglio1!$A$3,Foglio1!$A$23,Foglio1!$A$43,Foglio1!$A$63,Foglio1!$A$83,Foglio1!$A$103,Foglio1!$A$123)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">(Foglio1!$A$3,Foglio1!$A$23,Foglio1!$A$43,Foglio1!$A$63,Foglio1!$A$83,Foglio1!$A$103,Foglio1!$A$123)</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">(Foglio1!$A$3,Foglio1!$A$23,Foglio1!$A$43,Foglio1!$A$63,Foglio1!$A$83,Foglio1!$A$103,Foglio1!$A$123)</definedName>
-  </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -372,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -427,6 +422,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -811,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,7 +1269,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>67</v>
@@ -1286,10 +1282,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
-        <v>2.2999999999999998</v>
+        <v>14.5</v>
       </c>
       <c r="B23" s="29">
-        <v>81920</v>
+        <v>70656</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
@@ -1334,22 +1330,22 @@
         <v>9</v>
       </c>
       <c r="B25">
-        <v>0.19132855800000001</v>
-      </c>
-      <c r="C25">
-        <v>0.20249655799999999</v>
-      </c>
-      <c r="D25">
-        <v>0.199591558</v>
-      </c>
-      <c r="E25">
-        <v>0.19322655799999999</v>
+        <v>0.94881367750000001</v>
+      </c>
+      <c r="C25" s="16">
+        <v>1.0271606775</v>
+      </c>
+      <c r="D25" s="16">
+        <v>0.95294267749999995</v>
+      </c>
+      <c r="E25" s="16">
+        <v>0.96316767749999999</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="1">
-        <v>0.23316712114999999</v>
+        <v>1.1807083644</v>
       </c>
       <c r="H25" s="1">
         <v>0.34020732115000002</v>
@@ -1366,13 +1362,13 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>1142.105</v>
+        <v>1173.547</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="1">
-        <v>654.46500000000003</v>
+        <v>645.51599999999996</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>25</v>
@@ -1389,13 +1385,13 @@
         <v>15</v>
       </c>
       <c r="B27">
-        <v>8364.5159999999996</v>
+        <v>8375.223</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="1">
-        <v>1062.8399999999999</v>
+        <v>1160.2729999999999</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -1403,13 +1399,13 @@
         <v>16</v>
       </c>
       <c r="B28">
-        <v>1154.8869999999999</v>
+        <v>1203.8789999999999</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="15">
-        <v>659.42600000000004</v>
+      <c r="G28" s="1">
+        <v>673.50400000000002</v>
       </c>
       <c r="H28" s="15" t="s">
         <v>28</v>
@@ -1426,13 +1422,13 @@
         <v>19</v>
       </c>
       <c r="B29">
-        <v>8369.7379999999994</v>
+        <v>8439.223</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="15">
-        <v>1067.75</v>
+      <c r="G29" s="1">
+        <v>1188.191</v>
       </c>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
@@ -1443,13 +1439,13 @@
         <v>20</v>
       </c>
       <c r="B30">
-        <v>1249.6289999999999</v>
+        <v>1326.9880000000001</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G30" s="1">
-        <v>674.41800000000001</v>
+        <v>678.95699999999999</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -1457,13 +1453,13 @@
         <v>21</v>
       </c>
       <c r="B31">
-        <v>8532.7579999999998</v>
+        <v>8603.2420000000002</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G31" s="1">
-        <v>1128.1020000000001</v>
+        <v>1190.914</v>
       </c>
       <c r="M31" s="20"/>
     </row>
@@ -1472,22 +1468,22 @@
         <v>22</v>
       </c>
       <c r="B32" s="16">
-        <v>2.3769035219959798E-16</v>
+        <v>1.2477434442123901E-13</v>
       </c>
       <c r="C32" s="16">
-        <v>2.3769035219959798E-16</v>
+        <v>1.2477434442123901E-13</v>
       </c>
       <c r="D32" s="16">
-        <v>2.3769035219959798E-16</v>
+        <v>1.2477434442123901E-13</v>
       </c>
       <c r="E32" s="16">
-        <v>2.3769035219959798E-16</v>
+        <v>1.2477434442123901E-13</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="16">
-        <v>2.3769035219959699E-16</v>
+        <v>9.4510413200822E-14</v>
       </c>
       <c r="H32" s="17">
         <v>2.3769035219959699E-16</v>
@@ -1536,22 +1532,13 @@
         <v>9</v>
       </c>
       <c r="B34">
-        <v>3.5251380000000001</v>
-      </c>
-      <c r="C34">
-        <v>5.2649109999999997</v>
-      </c>
-      <c r="D34">
-        <v>5.3341580000000004</v>
-      </c>
-      <c r="E34">
-        <v>5.1598560000000004</v>
+        <v>142.35</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="15">
-        <v>2.9796689999999999</v>
+      <c r="G34" s="1">
+        <v>105.13113800000001</v>
       </c>
       <c r="K34" s="20"/>
     </row>
@@ -1560,22 +1547,13 @@
         <v>10</v>
       </c>
       <c r="B35">
-        <v>1908</v>
-      </c>
-      <c r="C35">
-        <v>1820</v>
-      </c>
-      <c r="D35">
-        <v>1908</v>
-      </c>
-      <c r="E35">
-        <v>1828</v>
+        <v>1824</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="1">
-        <v>3592</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1589,7 +1567,7 @@
         <v>15</v>
       </c>
       <c r="G36" s="1">
-        <v>908</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1597,22 +1575,13 @@
         <v>16</v>
       </c>
       <c r="B37">
-        <v>9296</v>
-      </c>
-      <c r="C37">
-        <v>9264</v>
-      </c>
-      <c r="D37">
-        <v>9288</v>
-      </c>
-      <c r="E37">
-        <v>9116</v>
+        <v>26568</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="15">
-        <v>7736</v>
+        <v>16164</v>
       </c>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
@@ -1623,13 +1592,13 @@
         <v>19</v>
       </c>
       <c r="B38">
-        <v>20008</v>
+        <v>37332</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G38" s="15">
-        <v>5780</v>
+        <v>13536</v>
       </c>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
@@ -1640,22 +1609,13 @@
         <v>20</v>
       </c>
       <c r="B39">
-        <v>39988</v>
-      </c>
-      <c r="C39">
-        <v>39892</v>
-      </c>
-      <c r="D39">
-        <v>39980</v>
-      </c>
-      <c r="E39">
-        <v>39872</v>
+        <v>464432</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G39" s="1">
-        <v>37124</v>
+        <v>442004</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -1663,13 +1623,13 @@
         <v>21</v>
       </c>
       <c r="B40">
-        <v>50896</v>
+        <v>475212</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G40" s="1">
-        <v>34332</v>
+        <v>440088</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -1677,22 +1637,16 @@
         <v>22</v>
       </c>
       <c r="B41" s="16">
-        <v>2.77912E-16</v>
-      </c>
-      <c r="C41" s="16">
-        <v>2.77912E-16</v>
-      </c>
-      <c r="D41" s="16">
-        <v>2.77912E-16</v>
-      </c>
-      <c r="E41" s="16">
-        <v>2.77912E-16</v>
-      </c>
+        <v>2.5291300000000001E-12</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
       <c r="F41" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G41" s="16">
-        <v>2.7793099999999998E-16</v>
+        <v>2.5257199999999999E-12</v>
       </c>
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
@@ -1700,7 +1654,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B42" s="25" t="s">
         <v>67</v>
@@ -1713,10 +1667,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
-        <v>8.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B43" s="29">
-        <v>715176</v>
+        <v>81920</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="25"/>
@@ -1761,22 +1715,22 @@
         <v>9</v>
       </c>
       <c r="B45">
-        <v>8.6413686774999992</v>
+        <v>0.19132855800000001</v>
       </c>
       <c r="C45">
-        <v>8.1384656774999993</v>
+        <v>0.20249655799999999</v>
       </c>
       <c r="D45">
-        <v>6.3027876774999996</v>
+        <v>0.199591558</v>
       </c>
       <c r="E45">
-        <v>5.9392856775</v>
+        <v>0.19322655799999999</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="1">
-        <v>7.1606706644000004</v>
+        <v>0.23316712114999999</v>
       </c>
       <c r="H45" s="1">
         <v>7.2193678643999997</v>
@@ -1793,13 +1747,13 @@
         <v>10</v>
       </c>
       <c r="B46">
-        <v>1111.934</v>
+        <v>1142.105</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="1">
-        <v>676.61300000000006</v>
+        <v>654.46500000000003</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>32</v>
@@ -1816,13 +1770,13 @@
         <v>15</v>
       </c>
       <c r="B47">
-        <v>8367.527</v>
+        <v>8364.5159999999996</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G47" s="1">
-        <v>1148.3320000000001</v>
+        <v>1062.8399999999999</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -1830,13 +1784,13 @@
         <v>16</v>
       </c>
       <c r="B48">
-        <v>1206.5899999999999</v>
+        <v>1154.8869999999999</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="15">
-        <v>756.00800000000004</v>
+        <v>659.42600000000004</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>35</v>
@@ -1853,13 +1807,13 @@
         <v>19</v>
       </c>
       <c r="B49">
-        <v>8446.2659999999996</v>
+        <v>8369.7379999999994</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G49" s="15">
-        <v>1227.652</v>
+        <v>1067.75</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -1867,13 +1821,13 @@
         <v>20</v>
       </c>
       <c r="B50">
-        <v>1363.172</v>
+        <v>1249.6289999999999</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G50" s="1">
-        <v>772.77</v>
+        <v>674.41800000000001</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -1881,13 +1835,13 @@
         <v>21</v>
       </c>
       <c r="B51">
-        <v>8673.2849999999999</v>
+        <v>8532.7579999999998</v>
       </c>
       <c r="F51" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G51" s="1">
-        <v>1244.3869999999999</v>
+        <v>1128.1020000000001</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -1895,22 +1849,22 @@
         <v>22</v>
       </c>
       <c r="B52" s="16">
-        <v>4.3712464003366997E-11</v>
+        <v>2.3769035219959798E-16</v>
       </c>
       <c r="C52" s="16">
-        <v>4.3712464003366997E-11</v>
+        <v>2.3769035219959798E-16</v>
       </c>
       <c r="D52" s="16">
-        <v>4.3712464003366997E-11</v>
+        <v>2.3769035219959798E-16</v>
       </c>
       <c r="E52" s="16">
-        <v>4.3712464003366997E-11</v>
+        <v>2.3769035219959798E-16</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G52" s="16">
-        <v>4.3741091793688501E-11</v>
+        <v>2.3769035219959699E-16</v>
       </c>
       <c r="H52" s="17">
         <v>4.3741091793688501E-11</v>
@@ -1959,13 +1913,22 @@
         <v>9</v>
       </c>
       <c r="B54">
-        <v>1792.4765400000001</v>
+        <v>3.5251380000000001</v>
+      </c>
+      <c r="C54">
+        <v>5.2649109999999997</v>
+      </c>
+      <c r="D54">
+        <v>5.3341580000000004</v>
+      </c>
+      <c r="E54">
+        <v>5.1598560000000004</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G54" s="1">
-        <v>1321.0058469999999</v>
+      <c r="G54" s="15">
+        <v>2.9796689999999999</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -1973,13 +1936,22 @@
         <v>10</v>
       </c>
       <c r="B55">
-        <v>1872</v>
+        <v>1908</v>
+      </c>
+      <c r="C55">
+        <v>1820</v>
+      </c>
+      <c r="D55">
+        <v>1908</v>
+      </c>
+      <c r="E55">
+        <v>1828</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G55" s="1">
-        <v>3600</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -1993,7 +1965,7 @@
         <v>15</v>
       </c>
       <c r="G56" s="1">
-        <v>916</v>
+        <v>908</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -2001,13 +1973,22 @@
         <v>16</v>
       </c>
       <c r="B57">
-        <v>55100</v>
+        <v>9296</v>
+      </c>
+      <c r="C57">
+        <v>9264</v>
+      </c>
+      <c r="D57">
+        <v>9288</v>
+      </c>
+      <c r="E57">
+        <v>9116</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G57" s="15">
-        <v>40120</v>
+        <v>7736</v>
       </c>
       <c r="H57" s="15"/>
       <c r="I57" s="15"/>
@@ -2018,13 +1999,13 @@
         <v>19</v>
       </c>
       <c r="B58">
-        <v>65860</v>
+        <v>20008</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G58" s="15">
-        <v>37276</v>
+        <v>5780</v>
       </c>
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
@@ -2035,13 +2016,22 @@
         <v>20</v>
       </c>
       <c r="B59">
-        <v>2716200</v>
+        <v>39988</v>
+      </c>
+      <c r="C59">
+        <v>39892</v>
+      </c>
+      <c r="D59">
+        <v>39980</v>
+      </c>
+      <c r="E59">
+        <v>39872</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G59" s="18">
-        <v>2630880</v>
+      <c r="G59" s="1">
+        <v>37124</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -2049,13 +2039,13 @@
         <v>21</v>
       </c>
       <c r="B60">
-        <v>2729776</v>
+        <v>50896</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G60" s="17">
-        <v>2679030</v>
+      <c r="G60" s="1">
+        <v>34332</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -2063,16 +2053,22 @@
         <v>22</v>
       </c>
       <c r="B61" s="16">
-        <v>7.65522E-11</v>
-      </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
+        <v>2.77912E-16</v>
+      </c>
+      <c r="C61" s="16">
+        <v>2.77912E-16</v>
+      </c>
+      <c r="D61" s="16">
+        <v>2.77912E-16</v>
+      </c>
+      <c r="E61" s="16">
+        <v>2.77912E-16</v>
+      </c>
       <c r="F61" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G61" s="16">
-        <v>7.6552000000000001E-11</v>
+        <v>2.7793099999999998E-16</v>
       </c>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
@@ -2080,7 +2076,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B62" s="25" t="s">
         <v>67</v>
@@ -2088,20 +2084,20 @@
       <c r="C62" s="25"/>
       <c r="D62" s="25"/>
       <c r="E62" s="25"/>
-      <c r="F62" s="26"/>
+      <c r="F62" s="6"/>
       <c r="G62" s="27"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
-        <v>13.4</v>
+        <v>23.7</v>
       </c>
       <c r="B63" s="29">
-        <v>525825</v>
+        <v>123440</v>
       </c>
       <c r="C63" s="25"/>
       <c r="D63" s="25"/>
       <c r="E63" s="25"/>
-      <c r="F63" s="26"/>
+      <c r="F63" s="6"/>
       <c r="G63" s="27"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -2141,22 +2137,22 @@
         <v>9</v>
       </c>
       <c r="B65">
-        <v>1.6961926775</v>
+        <v>2.1868166775</v>
       </c>
       <c r="C65" s="16">
-        <v>1.6782621775</v>
-      </c>
-      <c r="D65">
-        <v>1.6925146775</v>
-      </c>
-      <c r="E65">
-        <v>1.7039386775000001</v>
+        <v>2.1862206775000002</v>
+      </c>
+      <c r="D65" s="16">
+        <v>2.2231206774999999</v>
+      </c>
+      <c r="E65" s="16">
+        <v>2.1912646775</v>
       </c>
       <c r="F65" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G65" s="1">
-        <v>1.7010531644</v>
+        <v>2.8942993487500002</v>
       </c>
       <c r="H65" s="17">
         <v>1.6956039644000001</v>
@@ -2173,13 +2169,13 @@
         <v>10</v>
       </c>
       <c r="B66">
-        <v>1112.3869999999999</v>
+        <v>1191.348</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G66" s="1">
-        <v>668.96900000000005</v>
+        <v>623.36699999999996</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>39</v>
@@ -2196,13 +2192,13 @@
         <v>15</v>
       </c>
       <c r="B67">
-        <v>8355.5079999999998</v>
+        <v>8378.8709999999992</v>
       </c>
       <c r="F67" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G67" s="1">
-        <v>1154.453</v>
+        <v>1161.5509999999999</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -2210,13 +2206,13 @@
         <v>16</v>
       </c>
       <c r="B68">
-        <v>1199.9380000000001</v>
+        <v>1251.7070000000001</v>
       </c>
       <c r="F68" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G68" s="1">
-        <v>733.04700000000003</v>
+        <v>671.32</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>42</v>
@@ -2233,13 +2229,13 @@
         <v>19</v>
       </c>
       <c r="B69">
-        <v>8414.8089999999993</v>
+        <v>8425.9570000000003</v>
       </c>
       <c r="F69" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G69" s="1">
-        <v>1218.625</v>
+        <v>1208.6949999999999</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -2247,13 +2243,13 @@
         <v>20</v>
       </c>
       <c r="B70">
-        <v>1383.32</v>
+        <v>1351.5429999999999</v>
       </c>
       <c r="F70" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G70" s="1">
-        <v>745.19899999999996</v>
+        <v>679.31200000000001</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -2261,13 +2257,13 @@
         <v>21</v>
       </c>
       <c r="B71">
-        <v>8707.8279999999995</v>
+        <v>8653.9770000000008</v>
       </c>
       <c r="F71" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G71" s="1">
-        <v>1230.6130000000001</v>
+        <v>1216.1369999999999</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -2275,22 +2271,22 @@
         <v>22</v>
       </c>
       <c r="B72" s="16">
-        <v>1.09185181855155E-12</v>
+        <v>3.9266658070966701E-13</v>
       </c>
       <c r="C72" s="16">
-        <v>1.09185181855155E-12</v>
+        <v>3.9266658070966701E-13</v>
       </c>
       <c r="D72" s="16">
-        <v>1.09185181855155E-12</v>
+        <v>3.9266658070966701E-13</v>
       </c>
       <c r="E72" s="16">
-        <v>1.09185181855155E-12</v>
+        <v>3.9266658070966701E-13</v>
       </c>
       <c r="F72" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G72" s="16">
-        <v>1.08593319293648E-12</v>
+        <v>4.1297678306891098E-13</v>
       </c>
       <c r="H72" s="17">
         <v>1.08593319293648E-12</v>
@@ -2339,13 +2335,16 @@
         <v>9</v>
       </c>
       <c r="B74">
-        <v>77.029069000000007</v>
+        <v>640</v>
+      </c>
+      <c r="C74">
+        <v>635.26900000000001</v>
       </c>
       <c r="F74" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G74" s="1">
-        <v>55.008611000000002</v>
+        <v>334.02775800000001</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -2353,13 +2352,16 @@
         <v>10</v>
       </c>
       <c r="B75">
-        <v>1808</v>
+        <v>1964</v>
+      </c>
+      <c r="C75">
+        <v>1892</v>
       </c>
       <c r="F75" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G75" s="1">
-        <v>3636</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -2373,7 +2375,7 @@
         <v>15</v>
       </c>
       <c r="G76" s="1">
-        <v>996</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
@@ -2381,13 +2383,16 @@
         <v>16</v>
       </c>
       <c r="B77">
-        <v>42360</v>
+        <v>42508</v>
+      </c>
+      <c r="C77">
+        <v>42588</v>
       </c>
       <c r="F77" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G77" s="1">
-        <v>31612</v>
+      <c r="G77" s="15">
+        <v>24680</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
@@ -2395,27 +2400,30 @@
         <v>19</v>
       </c>
       <c r="B78">
-        <v>53232</v>
+        <v>53328</v>
       </c>
       <c r="F78" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G78" s="15">
-        <v>28800</v>
+        <v>22088</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B79" s="21">
-        <v>523956</v>
+      <c r="B79">
+        <v>913424</v>
+      </c>
+      <c r="C79">
+        <v>913448</v>
       </c>
       <c r="F79" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G79" s="15">
-        <v>477380</v>
+      <c r="G79" s="1">
+        <v>893140</v>
       </c>
       <c r="H79" s="15"/>
       <c r="I79" s="15"/>
@@ -2426,13 +2434,13 @@
         <v>21</v>
       </c>
       <c r="B80">
-        <v>534704</v>
+        <v>924128</v>
       </c>
       <c r="F80" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G80" s="1">
-        <v>475396</v>
+        <v>892568</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -2440,16 +2448,18 @@
         <v>22</v>
       </c>
       <c r="B81" s="16">
-        <v>2.7677E-12</v>
-      </c>
-      <c r="C81" s="16"/>
+        <v>5.5869100000000001E-12</v>
+      </c>
+      <c r="C81" s="16">
+        <v>5.5869100000000001E-12</v>
+      </c>
       <c r="D81" s="16"/>
       <c r="E81" s="16"/>
       <c r="F81" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G81" s="16">
-        <v>2.7692800000000001E-12</v>
+        <v>5.5792500000000001E-12</v>
       </c>
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
@@ -2458,7 +2468,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B82" s="25" t="s">
         <v>67</v>
@@ -2471,10 +2481,10 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
-        <v>14.2</v>
+        <v>13.4</v>
       </c>
       <c r="B83" s="29">
-        <v>1585478</v>
+        <v>525825</v>
       </c>
       <c r="C83" s="25"/>
       <c r="D83" s="25"/>
@@ -2519,22 +2529,22 @@
         <v>9</v>
       </c>
       <c r="B85">
-        <v>8.3968946775000006</v>
+        <v>1.6961926775</v>
       </c>
       <c r="C85" s="16">
-        <v>8.4139606775000004</v>
-      </c>
-      <c r="D85" s="16">
-        <v>8.4458086775000005</v>
-      </c>
-      <c r="E85" s="16">
-        <v>8.5108536775000001</v>
+        <v>1.6782621775</v>
+      </c>
+      <c r="D85">
+        <v>1.6925146775</v>
+      </c>
+      <c r="E85">
+        <v>1.7039386775000001</v>
       </c>
       <c r="F85" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G85" s="1">
-        <v>9.6780539644000001</v>
+        <v>1.7010531644</v>
       </c>
       <c r="H85" s="17">
         <v>15.652370664399999</v>
@@ -2551,13 +2561,13 @@
         <v>10</v>
       </c>
       <c r="B86">
-        <v>1135.1679999999999</v>
+        <v>1112.3869999999999</v>
       </c>
       <c r="F86" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G86" s="1">
-        <v>653.19500000000005</v>
+        <v>668.96900000000005</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>45</v>
@@ -2574,13 +2584,13 @@
         <v>15</v>
       </c>
       <c r="B87">
-        <v>8364.5159999999996</v>
+        <v>8355.5079999999998</v>
       </c>
       <c r="F87" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G87" s="1">
-        <v>1157.5820000000001</v>
+        <v>1154.453</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
@@ -2588,13 +2598,13 @@
         <v>16</v>
       </c>
       <c r="B88">
-        <v>1283.52</v>
+        <v>1199.9380000000001</v>
       </c>
       <c r="F88" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G88" s="1">
-        <v>782.27700000000004</v>
+        <v>733.04700000000003</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
@@ -2602,13 +2612,13 @@
         <v>19</v>
       </c>
       <c r="B89">
-        <v>8486.6370000000006</v>
+        <v>8414.8089999999993</v>
       </c>
       <c r="F89" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G89" s="1">
-        <v>1286.98</v>
+        <v>1218.625</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>46</v>
@@ -2625,13 +2635,13 @@
         <v>20</v>
       </c>
       <c r="B90">
-        <v>1442.8320000000001</v>
+        <v>1383.32</v>
       </c>
       <c r="F90" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G90" s="1">
-        <v>803.98400000000004</v>
+        <v>745.19899999999996</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
@@ -2639,13 +2649,13 @@
         <v>21</v>
       </c>
       <c r="B91">
-        <v>8713.6949999999997</v>
+        <v>8707.8279999999995</v>
       </c>
       <c r="F91" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G91" s="1">
-        <v>1322.277</v>
+        <v>1230.6130000000001</v>
       </c>
       <c r="L91" s="21"/>
     </row>
@@ -2654,22 +2664,22 @@
         <v>22</v>
       </c>
       <c r="B92" s="16">
-        <v>3.5205511727878099E-12</v>
+        <v>1.09185181855155E-12</v>
       </c>
       <c r="C92" s="16">
-        <v>3.5205511727878099E-12</v>
+        <v>1.09185181855155E-12</v>
       </c>
       <c r="D92" s="16">
-        <v>3.5205511727878099E-12</v>
+        <v>1.09185181855155E-12</v>
       </c>
       <c r="E92" s="16">
-        <v>3.5205511727878099E-12</v>
+        <v>1.09185181855155E-12</v>
       </c>
       <c r="F92" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G92" s="16">
-        <v>3.5231237702934399E-12</v>
+        <v>1.08593319293648E-12</v>
       </c>
       <c r="H92" s="17">
         <v>3.5231237702934399E-12</v>
@@ -2718,13 +2728,13 @@
         <v>9</v>
       </c>
       <c r="B94">
-        <v>841.00264600000003</v>
+        <v>77.029069000000007</v>
       </c>
       <c r="F94" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G94" s="1">
-        <v>633.13135</v>
+        <v>55.008611000000002</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
@@ -2732,13 +2742,13 @@
         <v>10</v>
       </c>
       <c r="B95">
-        <v>1892</v>
+        <v>1808</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G95" s="1">
-        <v>3648</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
@@ -2752,7 +2762,7 @@
         <v>15</v>
       </c>
       <c r="G96" s="1">
-        <v>1008</v>
+        <v>996</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
@@ -2760,13 +2770,13 @@
         <v>16</v>
       </c>
       <c r="B97">
-        <v>82420</v>
+        <v>42360</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G97" s="15">
-        <v>65320</v>
+      <c r="G97" s="1">
+        <v>31612</v>
       </c>
       <c r="H97" s="15"/>
       <c r="I97" s="15"/>
@@ -2777,13 +2787,13 @@
         <v>19</v>
       </c>
       <c r="B98">
-        <v>93204</v>
+        <v>53232</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G98" s="15">
-        <v>62572</v>
+        <v>28800</v>
       </c>
       <c r="H98" s="15"/>
       <c r="I98" s="15"/>
@@ -2793,14 +2803,14 @@
       <c r="A99" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B99">
-        <v>2148580</v>
+      <c r="B99" s="21">
+        <v>523956</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G99" s="17">
-        <v>2120600</v>
+      <c r="G99" s="15">
+        <v>477380</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
@@ -2808,13 +2818,13 @@
         <v>21</v>
       </c>
       <c r="B100">
-        <v>2165336</v>
+        <v>534704</v>
       </c>
       <c r="F100" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G100" s="17">
-        <v>2120600</v>
+      <c r="G100" s="1">
+        <v>475396</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
@@ -2822,7 +2832,7 @@
         <v>22</v>
       </c>
       <c r="B101" s="16">
-        <v>7.5734800000000002E-12</v>
+        <v>2.7677E-12</v>
       </c>
       <c r="C101" s="16"/>
       <c r="D101" s="16"/>
@@ -2831,7 +2841,7 @@
         <v>22</v>
       </c>
       <c r="G101" s="16">
-        <v>7.5720200000000007E-12</v>
+        <v>2.7692800000000001E-12</v>
       </c>
       <c r="H101" s="17"/>
       <c r="I101" s="17"/>
@@ -2839,7 +2849,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B102" s="25" t="s">
         <v>67</v>
@@ -2852,10 +2862,10 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
-        <v>14.5</v>
+        <v>8.5</v>
       </c>
       <c r="B103" s="29">
-        <v>70656</v>
+        <v>715176</v>
       </c>
       <c r="C103" s="25"/>
       <c r="D103" s="25"/>
@@ -2900,22 +2910,22 @@
         <v>9</v>
       </c>
       <c r="B105">
-        <v>0.94881367750000001</v>
-      </c>
-      <c r="C105" s="16">
-        <v>1.0271606775</v>
-      </c>
-      <c r="D105" s="16">
-        <v>0.95294267749999995</v>
-      </c>
-      <c r="E105" s="16">
-        <v>0.96316767749999999</v>
+        <v>8.6413686774999992</v>
+      </c>
+      <c r="C105">
+        <v>8.1384656774999993</v>
+      </c>
+      <c r="D105">
+        <v>6.3027876774999996</v>
+      </c>
+      <c r="E105">
+        <v>5.9392856775</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G105" s="1">
-        <v>1.1807083644</v>
+        <v>7.1606706644000004</v>
       </c>
       <c r="H105" s="17">
         <v>1.2784996644</v>
@@ -2932,13 +2942,13 @@
         <v>10</v>
       </c>
       <c r="B106">
-        <v>1173.547</v>
+        <v>1111.934</v>
       </c>
       <c r="F106" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G106" s="1">
-        <v>645.51599999999996</v>
+        <v>676.61300000000006</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>49</v>
@@ -2955,13 +2965,13 @@
         <v>15</v>
       </c>
       <c r="B107">
-        <v>8375.223</v>
+        <v>8367.527</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G107" s="1">
-        <v>1160.2729999999999</v>
+        <v>1148.3320000000001</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
@@ -2969,13 +2979,13 @@
         <v>16</v>
       </c>
       <c r="B108">
-        <v>1203.8789999999999</v>
+        <v>1206.5899999999999</v>
       </c>
       <c r="F108" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G108" s="1">
-        <v>673.50400000000002</v>
+      <c r="G108" s="15">
+        <v>756.00800000000004</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>50</v>
@@ -2992,13 +3002,13 @@
         <v>19</v>
       </c>
       <c r="B109">
-        <v>8439.223</v>
+        <v>8446.2659999999996</v>
       </c>
       <c r="F109" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G109" s="1">
-        <v>1188.191</v>
+      <c r="G109" s="15">
+        <v>1227.652</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
@@ -3006,13 +3016,13 @@
         <v>20</v>
       </c>
       <c r="B110">
-        <v>1326.9880000000001</v>
+        <v>1363.172</v>
       </c>
       <c r="F110" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G110" s="1">
-        <v>678.95699999999999</v>
+        <v>772.77</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
@@ -3020,13 +3030,13 @@
         <v>21</v>
       </c>
       <c r="B111">
-        <v>8603.2420000000002</v>
+        <v>8673.2849999999999</v>
       </c>
       <c r="F111" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G111" s="1">
-        <v>1190.914</v>
+        <v>1244.3869999999999</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
@@ -3034,22 +3044,22 @@
         <v>22</v>
       </c>
       <c r="B112" s="16">
-        <v>1.2477434442123901E-13</v>
+        <v>4.3712464003366997E-11</v>
       </c>
       <c r="C112" s="16">
-        <v>1.2477434442123901E-13</v>
+        <v>4.3712464003366997E-11</v>
       </c>
       <c r="D112" s="16">
-        <v>1.2477434442123901E-13</v>
+        <v>4.3712464003366997E-11</v>
       </c>
       <c r="E112" s="16">
-        <v>1.2477434442123901E-13</v>
+        <v>4.3712464003366997E-11</v>
       </c>
       <c r="F112" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G112" s="16">
-        <v>9.4510413200822E-14</v>
+        <v>4.3741091793688501E-11</v>
       </c>
       <c r="H112" s="17">
         <v>9.4510413200822E-14</v>
@@ -3098,13 +3108,13 @@
         <v>9</v>
       </c>
       <c r="B114">
-        <v>142.35</v>
+        <v>1792.4765400000001</v>
       </c>
       <c r="F114" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G114" s="1">
-        <v>105.13113800000001</v>
+        <v>1321.0058469999999</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
@@ -3112,13 +3122,13 @@
         <v>10</v>
       </c>
       <c r="B115">
-        <v>1824</v>
+        <v>1872</v>
       </c>
       <c r="F115" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G115" s="1">
-        <v>3640</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
@@ -3132,7 +3142,7 @@
         <v>15</v>
       </c>
       <c r="G116" s="1">
-        <v>1000</v>
+        <v>916</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
@@ -3140,13 +3150,13 @@
         <v>16</v>
       </c>
       <c r="B117">
-        <v>26568</v>
+        <v>55100</v>
       </c>
       <c r="F117" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G117" s="15">
-        <v>16164</v>
+        <v>40120</v>
       </c>
       <c r="H117" s="15"/>
       <c r="I117" s="15"/>
@@ -3157,13 +3167,13 @@
         <v>19</v>
       </c>
       <c r="B118">
-        <v>37332</v>
+        <v>65860</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G118" s="15">
-        <v>13536</v>
+        <v>37276</v>
       </c>
       <c r="H118" s="15"/>
       <c r="I118" s="15"/>
@@ -3174,13 +3184,13 @@
         <v>20</v>
       </c>
       <c r="B119">
-        <v>464432</v>
+        <v>2716200</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G119" s="1">
-        <v>442004</v>
+      <c r="G119" s="18">
+        <v>2630880</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
@@ -3188,13 +3198,13 @@
         <v>21</v>
       </c>
       <c r="B120">
-        <v>475212</v>
+        <v>2729776</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G120" s="1">
-        <v>440088</v>
+      <c r="G120" s="17">
+        <v>2679030</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
@@ -3202,7 +3212,7 @@
         <v>22</v>
       </c>
       <c r="B121" s="16">
-        <v>2.5291300000000001E-12</v>
+        <v>7.65522E-11</v>
       </c>
       <c r="C121" s="16"/>
       <c r="D121" s="16"/>
@@ -3211,7 +3221,7 @@
         <v>22</v>
       </c>
       <c r="G121" s="16">
-        <v>2.5257199999999999E-12</v>
+        <v>7.6552000000000001E-11</v>
       </c>
       <c r="H121" s="17"/>
       <c r="I121" s="17"/>
@@ -3219,7 +3229,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B122" s="25" t="s">
         <v>67</v>
@@ -3227,20 +3237,20 @@
       <c r="C122" s="25"/>
       <c r="D122" s="25"/>
       <c r="E122" s="25"/>
-      <c r="F122" s="6"/>
+      <c r="F122" s="26"/>
       <c r="G122" s="27"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
-        <v>23.7</v>
+        <v>14.2</v>
       </c>
       <c r="B123" s="29">
-        <v>123440</v>
+        <v>1585478</v>
       </c>
       <c r="C123" s="25"/>
       <c r="D123" s="25"/>
       <c r="E123" s="25"/>
-      <c r="F123" s="6"/>
+      <c r="F123" s="26"/>
       <c r="G123" s="27"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
@@ -3280,22 +3290,22 @@
         <v>9</v>
       </c>
       <c r="B125">
-        <v>2.1868166775</v>
+        <v>8.3968946775000006</v>
       </c>
       <c r="C125" s="16">
-        <v>2.1862206775000002</v>
+        <v>8.4139606775000004</v>
       </c>
       <c r="D125" s="16">
-        <v>2.2231206774999999</v>
+        <v>8.4458086775000005</v>
       </c>
       <c r="E125" s="16">
-        <v>2.1912646775</v>
+        <v>8.5108536775000001</v>
       </c>
       <c r="F125" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G125" s="1">
-        <v>2.8942993487500002</v>
+        <v>9.6780539644000001</v>
       </c>
       <c r="H125" s="17">
         <v>2.9954103987499998</v>
@@ -3312,13 +3322,13 @@
         <v>10</v>
       </c>
       <c r="B126">
-        <v>1191.348</v>
+        <v>1135.1679999999999</v>
       </c>
       <c r="F126" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G126" s="1">
-        <v>623.36699999999996</v>
+        <v>653.19500000000005</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>54</v>
@@ -3335,13 +3345,13 @@
         <v>15</v>
       </c>
       <c r="B127">
-        <v>8378.8709999999992</v>
+        <v>8364.5159999999996</v>
       </c>
       <c r="F127" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G127" s="1">
-        <v>1161.5509999999999</v>
+        <v>1157.5820000000001</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.3">
@@ -3349,13 +3359,13 @@
         <v>16</v>
       </c>
       <c r="B128">
-        <v>1251.7070000000001</v>
+        <v>1283.52</v>
       </c>
       <c r="F128" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G128" s="1">
-        <v>671.32</v>
+        <v>782.27700000000004</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>57</v>
@@ -3372,13 +3382,13 @@
         <v>19</v>
       </c>
       <c r="B129">
-        <v>8425.9570000000003</v>
+        <v>8486.6370000000006</v>
       </c>
       <c r="F129" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G129" s="1">
-        <v>1208.6949999999999</v>
+        <v>1286.98</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.3">
@@ -3386,13 +3396,13 @@
         <v>20</v>
       </c>
       <c r="B130">
-        <v>1351.5429999999999</v>
+        <v>1442.8320000000001</v>
       </c>
       <c r="F130" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G130" s="1">
-        <v>679.31200000000001</v>
+        <v>803.98400000000004</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.3">
@@ -3400,13 +3410,13 @@
         <v>21</v>
       </c>
       <c r="B131">
-        <v>8653.9770000000008</v>
+        <v>8713.6949999999997</v>
       </c>
       <c r="F131" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G131" s="1">
-        <v>1216.1369999999999</v>
+        <v>1322.277</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
@@ -3414,22 +3424,22 @@
         <v>22</v>
       </c>
       <c r="B132" s="16">
-        <v>3.9266658070966701E-13</v>
+        <v>3.5205511727878099E-12</v>
       </c>
       <c r="C132" s="16">
-        <v>3.9266658070966701E-13</v>
+        <v>3.5205511727878099E-12</v>
       </c>
       <c r="D132" s="16">
-        <v>3.9266658070966701E-13</v>
+        <v>3.5205511727878099E-12</v>
       </c>
       <c r="E132" s="16">
-        <v>3.9266658070966701E-13</v>
+        <v>3.5205511727878099E-12</v>
       </c>
       <c r="F132" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G132" s="16">
-        <v>4.1297678306891098E-13</v>
+        <v>3.5231237702934399E-12</v>
       </c>
       <c r="H132" s="17">
         <v>4.1297678306891098E-13</v>
@@ -3478,16 +3488,13 @@
         <v>9</v>
       </c>
       <c r="B134">
-        <v>640</v>
-      </c>
-      <c r="C134">
-        <v>635.26900000000001</v>
+        <v>841.00264600000003</v>
       </c>
       <c r="F134" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G134" s="1">
-        <v>334.02775800000001</v>
+        <v>633.13135</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.3">
@@ -3495,16 +3502,13 @@
         <v>10</v>
       </c>
       <c r="B135">
-        <v>1964</v>
-      </c>
-      <c r="C135">
         <v>1892</v>
       </c>
       <c r="F135" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G135" s="1">
-        <v>3640</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.3">
@@ -3518,7 +3522,7 @@
         <v>15</v>
       </c>
       <c r="G136" s="1">
-        <v>1004</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
@@ -3526,16 +3530,13 @@
         <v>16</v>
       </c>
       <c r="B137">
-        <v>42508</v>
-      </c>
-      <c r="C137">
-        <v>42588</v>
+        <v>82420</v>
       </c>
       <c r="F137" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G137" s="15">
-        <v>24680</v>
+        <v>65320</v>
       </c>
       <c r="H137" s="15"/>
       <c r="I137" s="15"/>
@@ -3546,13 +3547,13 @@
         <v>19</v>
       </c>
       <c r="B138">
-        <v>53328</v>
+        <v>93204</v>
       </c>
       <c r="F138" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G138" s="15">
-        <v>22088</v>
+        <v>62572</v>
       </c>
       <c r="H138" s="15"/>
       <c r="I138" s="15"/>
@@ -3563,16 +3564,13 @@
         <v>20</v>
       </c>
       <c r="B139">
-        <v>913424</v>
-      </c>
-      <c r="C139">
-        <v>913448</v>
+        <v>2148580</v>
       </c>
       <c r="F139" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G139" s="1">
-        <v>893140</v>
+      <c r="G139" s="17">
+        <v>2120600</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.3">
@@ -3580,13 +3578,13 @@
         <v>21</v>
       </c>
       <c r="B140">
-        <v>924128</v>
+        <v>2165336</v>
       </c>
       <c r="F140" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G140" s="1">
-        <v>892568</v>
+      <c r="G140" s="17">
+        <v>2120600</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.3">
@@ -3594,18 +3592,16 @@
         <v>22</v>
       </c>
       <c r="B141" s="16">
-        <v>5.5869100000000001E-12</v>
-      </c>
-      <c r="C141" s="16">
-        <v>5.5869100000000001E-12</v>
-      </c>
+        <v>7.5734800000000002E-12</v>
+      </c>
+      <c r="C141" s="16"/>
       <c r="D141" s="16"/>
       <c r="E141" s="16"/>
       <c r="F141" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G141" s="16">
-        <v>5.5792500000000001E-12</v>
+        <v>7.5720200000000007E-12</v>
       </c>
       <c r="H141" s="17"/>
       <c r="I141" s="17"/>
@@ -3624,7 +3620,7 @@
       <c r="H142" s="23"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A143" s="6">
+      <c r="A143" s="30">
         <v>182.6</v>
       </c>
       <c r="B143" s="22" t="s">

</xml_diff>

<commit_message>
updated memory plots and created presentation file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carloradice\Documents\MCSLinearSystemSolver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFE1029-288A-4610-8E49-894662F679B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E863D81-D6E3-4113-AD9E-FEFB3D942685}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="68">
   <si>
     <t xml:space="preserve">Ubuntu </t>
   </si>
@@ -235,7 +235,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -266,8 +266,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +335,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -367,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -423,6 +436,8 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -807,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,7 +854,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -864,6 +879,10 @@
       <c r="E3" s="25"/>
       <c r="F3" s="26"/>
       <c r="G3" s="27"/>
+      <c r="L3" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
@@ -933,7 +952,7 @@
         <v>1.580862115E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
@@ -960,7 +979,7 @@
       </c>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
@@ -1127,7 +1146,7 @@
         <v>0.117758</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>10</v>
       </c>
@@ -1150,7 +1169,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
@@ -1357,7 +1376,7 @@
         <v>0.14555462115000001</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>10</v>
       </c>
@@ -1380,7 +1399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>15</v>
       </c>
@@ -1542,7 +1561,7 @@
       </c>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>10</v>
       </c>
@@ -1556,7 +1575,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>15</v>
       </c>
@@ -1742,7 +1761,7 @@
         <v>7.2613738644000003</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>10</v>
       </c>
@@ -1765,7 +1784,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>15</v>
       </c>
@@ -1931,7 +1950,7 @@
         <v>2.9796689999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>10</v>
       </c>
@@ -1954,7 +1973,7 @@
         <v>3592</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>15</v>
       </c>
@@ -2164,7 +2183,7 @@
         <v>1.7020198644</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>10</v>
       </c>
@@ -2187,7 +2206,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
         <v>15</v>
       </c>
@@ -2347,7 +2366,7 @@
         <v>334.02775800000001</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
         <v>10</v>
       </c>
@@ -2364,7 +2383,7 @@
         <v>3640</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>15</v>
       </c>
@@ -2556,7 +2575,7 @@
         <v>10.3519378644</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
         <v>10</v>
       </c>
@@ -2579,7 +2598,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
         <v>15</v>
       </c>
@@ -2737,7 +2756,7 @@
         <v>55.008611000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
         <v>10</v>
       </c>
@@ -2751,7 +2770,7 @@
         <v>3636</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
         <v>15</v>
       </c>
@@ -2937,7 +2956,7 @@
         <v>1.1704009644</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
         <v>10</v>
       </c>
@@ -2960,7 +2979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
         <v>15</v>
       </c>
@@ -3117,7 +3136,7 @@
         <v>1321.0058469999999</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
         <v>10</v>
       </c>
@@ -3131,7 +3150,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12" t="s">
         <v>15</v>
       </c>
@@ -3317,7 +3336,7 @@
         <v>2.9556006987500001</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="12" t="s">
         <v>10</v>
       </c>
@@ -3340,7 +3359,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
         <v>15</v>
       </c>
@@ -3497,7 +3516,7 @@
         <v>633.13135</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="12" t="s">
         <v>10</v>
       </c>
@@ -3511,7 +3530,7 @@
         <v>3648</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="12" t="s">
         <v>15</v>
       </c>

</xml_diff>